<commit_message>
Update README file and configure swagger
</commit_message>
<xml_diff>
--- a/database/Atlanta Tigers Game data.xlsx
+++ b/database/Atlanta Tigers Game data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="28">
   <si>
     <t>PlayerId</t>
   </si>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t>Sophmore</t>
+  </si>
+  <si>
+    <t>2023-01-13</t>
+  </si>
+  <si>
+    <t>string</t>
   </si>
 </sst>
 </file>
@@ -424,7 +430,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M780"/>
+  <dimension ref="A1:M782"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
@@ -5008,11 +5014,87 @@
         <v>25</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="16"/>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="16"/>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>20</v>
+      </c>
+      <c r="B113" t="s">
+        <v>26</v>
+      </c>
+      <c r="C113" t="s">
+        <v>27</v>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+      <c r="E113">
+        <v>0</v>
+      </c>
+      <c r="F113">
+        <v>0</v>
+      </c>
+      <c r="G113">
+        <v>0</v>
+      </c>
+      <c r="H113">
+        <v>0</v>
+      </c>
+      <c r="I113">
+        <v>0</v>
+      </c>
+      <c r="J113">
+        <v>0</v>
+      </c>
+      <c r="K113">
+        <v>0</v>
+      </c>
+      <c r="L113">
+        <v>0</v>
+      </c>
+      <c r="M113" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>90</v>
+      </c>
+      <c r="B114" t="s">
+        <v>24</v>
+      </c>
+      <c r="C114" t="s">
+        <v>19</v>
+      </c>
+      <c r="D114">
+        <v>0.33</v>
+      </c>
+      <c r="E114">
+        <v>3</v>
+      </c>
+      <c r="F114">
+        <v>3</v>
+      </c>
+      <c r="G114">
+        <v>0</v>
+      </c>
+      <c r="H114">
+        <v>1</v>
+      </c>
+      <c r="I114">
+        <v>2</v>
+      </c>
+      <c r="J114">
+        <v>1</v>
+      </c>
+      <c r="K114">
+        <v>0</v>
+      </c>
+      <c r="L114">
+        <v>0</v>
+      </c>
+      <c r="M114" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="16"/>
@@ -7011,6 +7093,12 @@
     </row>
     <row r="780" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A780" s="16"/>
+    </row>
+    <row r="781" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A781" s="16"/>
+    </row>
+    <row r="782" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A782" s="16"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>